<commit_message>
Updated Jim Cost Analysis. It is less expensive! :D!
</commit_message>
<xml_diff>
--- a/Electronics/Jim Cost Analysis.xlsx
+++ b/Electronics/Jim Cost Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Items</t>
   </si>
@@ -98,18 +98,6 @@
     <t>Female Midi Plug</t>
   </si>
   <si>
-    <t>LX0508</t>
-  </si>
-  <si>
-    <t>5V 8A power supply</t>
-  </si>
-  <si>
-    <t>Digi Key</t>
-  </si>
-  <si>
-    <t>2.5mm Female Power cable assembly</t>
-  </si>
-  <si>
     <t>USB to MIDI cable</t>
   </si>
   <si>
@@ -144,6 +132,12 @@
   </si>
   <si>
     <t>1x3 2.54mm Through Hole Headers</t>
+  </si>
+  <si>
+    <t>5V 10A power supply</t>
+  </si>
+  <si>
+    <t>JC0510</t>
   </si>
 </sst>
 </file>
@@ -183,18 +177,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -330,8 +318,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H26" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:H25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H25" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:H24"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Items" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="7"/>
     <tableColumn id="2" name="Part Number" dataDxfId="14" totalsRowDxfId="6" dataCellStyle="Hyperlink"/>
@@ -615,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -664,12 +652,12 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/TE-Connectivity/1-2199298-5?qs=sGAEpiMZZMs%2FSh%2Fkjph1tg2rzwRe0qPTk6j11BRLpRw%3D", "1-2199298-5")</f>
@@ -686,16 +674,16 @@
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <f>IF(E2 &lt; 10, 1.4, IF(E2 &lt; 100, 1.27, IF(E2 &lt; 500, 1.2, IF(E2 &lt; 1000, 1.14, IF(E2 &lt; 5000, 1.09, IF(E2 &lt; 10000, 0.985, 0.906))))))</f>
-        <v>1.4</v>
+        <f>IF(E2 &lt; 10, 0.28, IF(E2 &lt; 100, 0.216, IF(E2 &lt; 500, 0.186, IF(E2 &lt; 1000, 0.162, IF(E2 &lt; 2500, 0.135, IF(E2 &lt; 5000, 0.123, 0.116))))))</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G2" s="3">
         <f>F2*D2</f>
-        <v>1.4</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H2" s="3">
         <f>F2*E2</f>
-        <v>1.4</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
@@ -703,7 +691,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Microchip-Technology/PIC16F628A-I-P?qs=sGAEpiMZZMvqv2n3s2xjsbeKtMLkSi%252B7%2Fs4CDSEeoLU%3D", "PIC16F628A-I/P")</f>
@@ -716,19 +704,19 @@
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E25" si="0">J$2*D3</f>
+        <f t="shared" ref="E3:E24" si="0">J$2*D3</f>
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <f>IF(E3 &lt; 10, 1.78, IF(E3 &lt; 25, 1.63, IF(E3 &lt; 100, 1.45, 1.31)))</f>
+        <f>IF(E3 &lt; 10, 1.78, IF(E3 &lt; 25, 1.75, 1.72))</f>
         <v>1.78</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G25" si="1">F3*D3</f>
+        <f t="shared" ref="G3:G24" si="1">F3*D3</f>
         <v>1.78</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H25" si="2">F3*E3</f>
+        <f t="shared" ref="H3:H24" si="2">F3*E3</f>
         <v>1.78</v>
       </c>
     </row>
@@ -751,21 +739,21 @@
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <f>IF(E4 &lt; 10, 0.1, IF(E4 &lt; 100, 0.09, IF(E4 &lt; 1000, 0.08, IF(E4 &lt; 2500, 0.07, 0.069))))</f>
-        <v>0.1</v>
+        <f>IF(E4 &lt; 10, 0.22, IF(E4 &lt; 100, 0.175, IF(E4 &lt; 500, 0.135, IF(E4 &lt; 1000, 0.12, IF(E4 &lt; 2500, 0.099, IF(E4 &lt; 5000, 0.09, IF(E4 &lt; 10000, 0.088, 0.08)))))))</f>
+        <v>0.22</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Lite-On/6N138M?qs=sGAEpiMZZMtd3yBnp8bAgJVeHfvx%252b1RWDaKIx5bH5CM%3d", "6N138M")</f>
@@ -813,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <f>IF(E6 &lt; 50, 0.1, IF(E6 &lt; 100, 0.054, IF(E6 &lt; 1000, 0.044, IF(E6 &lt; 5000, 0.04, IF(E6 &lt; 30000, 0.033, IF(E6 &lt; 50000, 0.03, 0.028))))))</f>
+        <f>IF(E6 &lt; 50, 0.1, IF(E6 &lt; 100, 0.054, IF(E6 &lt; 1000, 0.044, IF(E6 &lt; 5000, 0.04, 0.033))))</f>
         <v>0.1</v>
       </c>
       <c r="G6" s="3">
@@ -875,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="3">
-        <f>IF(E8 &lt; 10, 0.26, IF(E8 &lt; 100, 0.207, IF(E8 &lt; 500, 0.184, IF(E8 &lt; 1000, 0.149, IF(E8 &lt; 2000, 0.138, IF(E8 &lt; 5000, 0.112, IF(E8 &lt; 10000, 0.096, IF(E8 &lt; 25000, 0.081, 0.074))))))))</f>
+        <f>IF(E8 &lt; 10, 0.26, IF(E8 &lt; 100, 0.207, IF(E8 &lt; 25000, 0.184, 0.182)))</f>
         <v>0.26</v>
       </c>
       <c r="G8" s="3">
@@ -906,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="3">
-        <f>IF(E9 &lt; 10, 0.1, IF(E9 &lt; 100, 0.036, IF(E9 &lt; 1000, 0.012, IF(E9 &lt; 5000, 0.009, IF(E9 &lt; 10000, 0.007, IF(E9 &lt; 25000, 0.006, 0.005))))))</f>
+        <f>IF(E9 &lt; 10, 0.1, IF(E9 &lt; 100, 0.05, IF(E9 &lt; 1000, 0.018, IF(E9 &lt; 5000, 0.013, IF(E9 &lt; 10000, 0.01, 0.008)))))</f>
         <v>0.1</v>
       </c>
       <c r="G9" s="3">
@@ -937,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="3">
-        <f>IF(E10 &lt; 10, 0.1, IF(E10 &lt; 100, 0.036, IF(E10 &lt; 1000, 0.012, IF(E10 &lt; 5000, 0.009, IF(E10 &lt; 10000, 0.007, IF(E10 &lt; 25000, 0.006, 0.005))))))</f>
+        <f>IF(E10 &lt; 10, 0.1, IF(E10 &lt; 100, 0.05, IF(E10 &lt; 1000, 0.018, IF(E10 &lt; 5000, 0.013, IF(E10 &lt; 10000, 0.001, 0.008)))))</f>
         <v>0.1</v>
       </c>
       <c r="G10" s="3">
@@ -968,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <f>IF(E11 &lt; 10, 0.1, IF(E11 &lt; 100, 0.036, IF(E11 &lt; 1000, 0.012, IF(E11 &lt; 5000, 0.009, IF(E11 &lt; 10000, 0.007, IF(E11 &lt; 25000, 0.006, 0.005))))))</f>
+        <f>IF(E11 &lt; 10, 0.1, IF(E11 &lt; 100, 0.036, IF(E11 &lt; 1000, 0.012, IF(E11 &lt; 10000, 0.009, IF(E11 &lt; 50000, 0.008, 0.007)))))</f>
         <v>0.1</v>
       </c>
       <c r="G11" s="3">
@@ -999,16 +987,16 @@
         <v>1</v>
       </c>
       <c r="F12" s="3">
-        <f>IF(E12 &lt; 10, 0.1, IF(E12 &lt; 100, 0.08, IF(E12 &lt; 1000, 0.032, IF(E12 &lt; 5000, 0.015, IF(E12 &lt; 10000, 0.011, IF(E12 &lt; 25000, 0.01, IF(E12 &lt; 100000, 0.009, 0.008)))))))</f>
-        <v>0.1</v>
+        <f>IF(E12 &lt; 10, 0.12, IF(E12 &lt; 100, 0.063, IF(E12 &lt; 1000, 0.022, IF(E12 &lt; 5000, 0.016, IF(E12 &lt; 10000, 0.011, IF(E12 &lt; 25000, 0.01, IF(E12 &lt; 100000, 0.009, 0.008)))))))</f>
+        <v>0.12</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1030,16 +1018,16 @@
         <v>1</v>
       </c>
       <c r="F13" s="3">
-        <f>IF(E13 &lt; 10, 0.1, IF(E13 &lt; 100, 0.08, IF(E13 &lt; 1000, 0.032, IF(E13 &lt; 5000, 0.015, IF(E13 &lt; 10000, 0.011, IF(E13 &lt; 25000, 0.01, IF(E13 &lt; 100000, 0.009, 0.008)))))))</f>
-        <v>0.1</v>
+        <f>IF(E13 &lt; 10, 0.12, IF(E13 &lt; 100, 0.063, IF(E13 &lt; 1000, 0.0322, IF(E13 &lt; 5000, 0.016, IF(E13 &lt; 10000, 0.011, IF(E13 &lt; 25000, 0.01, IF(E13 &lt; 100000, 0.009, 0.008)))))))</f>
+        <v>0.12</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1061,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="3">
-        <f>IF(E14 &lt; 10, 0.1, IF(E14 &lt; 100, 0.036, IF(E14 &lt; 1000, 0.012, IF(E14 &lt; 5000, 0.009, IF(E14 &lt; 10000, 0.007, IF(E14 &lt; 25000, 0.006, 0.005))))))</f>
+        <f>IF(E14 &lt; 10, 0.1, IF(E14 &lt; 100, 0.05, IF(E14 &lt; 1000, 0.018, IF(E14 &lt; 5000, 0.013, IF(E14 &lt; 10000, 0.01, 0.008)))))</f>
         <v>0.1</v>
       </c>
       <c r="G14" s="3">
@@ -1092,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="3">
-        <f>IF(E15 &lt; 10, 0.1, IF(E15 &lt; 100, 0.036, IF(E15 &lt; 1000, 0.012, IF(E15 &lt; 5000, 0.009, IF(E15 &lt; 10000, 0.007, IF(E15 &lt; 25000, 0.006, 0.005))))))</f>
+        <f>IF(E15 &lt; 10, 0.1, IF(E15 &lt; 100, 0.05, IF(E15 &lt; 1000, 0.018, IF(E15 &lt; 5000, 0.013, IF(E15 &lt; 10000, 0.01, 0.008)))))</f>
         <v>0.1</v>
       </c>
       <c r="G15" s="3">
@@ -1106,7 +1094,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Rectron/1N4148-T?qs=sGAEpiMZZMtoHjESLttvkr6EjNfTfTJYVe0iDtoqTpQ%3d", "1N4148-T")</f>
@@ -1123,19 +1111,19 @@
         <v>1</v>
       </c>
       <c r="F16" s="3">
-        <f>IF(E16 &lt; 25, 0.03, IF(E16 &lt; 500, 0.02, IF(E16 &lt; 1000, 0.017, IF(E16 &lt; 2000, 0.014, IF(E16 &lt; 5000, 0.012, IF(E16 &lt; 10000, 0.011, 0.009))))))</f>
-        <v>0.03</v>
+        <f>IF(E16 &lt; 25, 0.1, IF(E16 &lt; 500, 0.023, IF(E16 &lt; 1000, 0.019, IF(E16 &lt; 2000, 0.016, IF(E16 &lt; 5000, 0.014, IF(E16 &lt; 10000, 0.013, 0.01))))))</f>
+        <v>0.1</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="1"/>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="2"/>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1157,16 +1145,16 @@
         <v>1</v>
       </c>
       <c r="F17" s="3">
-        <f>IF(E17 &lt; 10, 0.18, IF(E17 &lt; 100, 0.154, IF(E17 &lt; 1000, 0.054, IF(E17 &lt; 5000, 0.037, IF(E17 &lt; 10000, 0.028, IF(E17 &lt; 20000, 0.024, IF(E17 &lt; 40000, 0.022, IF(E17 &lt; 100000, 0.019, 0.016))))))))</f>
-        <v>0.18</v>
+        <f>IF(E17 &lt; 10, 0.19, IF(E17 &lt; 100, 0.161, IF(E17 &lt; 1000, 0.055, IF(E17 &lt; 2500, 0.032, IF(E17 &lt; 10000, 0.028, IF(E17 &lt; 20000, 0.025, IF(E17 &lt; 40000, 0.022, IF(E17 &lt; 100000, 0.02, 0.016))))))))</f>
+        <v>0.19</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="1"/>
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="2"/>
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1202,7 +1190,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/TE-Connectivity-AMP/103239-3?qs=sGAEpiMZZMs%252bGHln7q6pm48SVpWlpfsE4E5prxpv59w%3d", "103239-3")</f>
@@ -1219,16 +1207,16 @@
         <v>6</v>
       </c>
       <c r="F19" s="3">
-        <f>IF(E19 &lt; 100, 0.24, IF(E19 &lt; 500, 0.193, IF(E19 &lt; 1000, 0.189, IF(E19 &lt; 2000, 0.174, IF(E19 &lt; 5000, 0.17, IF(E19 &lt; 10000, 0.165, IF(E19 &lt; 25000, 0.16, IF(E19 &lt; 50000, 0.154, 0.149))))))))</f>
-        <v>0.24</v>
+        <f>IF(E19 &lt; 10, 0.45, IF(E19 &lt; 100, 0.316, IF(E19 &lt; 500, 0.304, IF(E19 &lt; 1000, 0.261, IF(E19 &lt; 2500, 0.217, IF(E19 &lt; 10000, 0.199, IF(E19 &lt; 25000, 0.174, IF(E19 &lt; 50000, 0.164, 0.159))))))))</f>
+        <v>0.45</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="1"/>
-        <v>1.44</v>
+        <v>2.7</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="2"/>
-        <v>1.44</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1294,13 +1282,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f>HYPERLINK("https://www.amazon.com/NEWSTYLE-Supply-Converter-Adapter-5-5x2-1mm/dp/B00MHV7576/ref=sr_1_4?ie=UTF8&amp;qid=1519886729&amp;sr=8-4&amp;keywords=5v+8a+power+supply", "Amazon")</f>
+        <f>HYPERLINK("https://www.amazon.com/dp/B07CMM2BBR/ref=dp_cerb_2", "Amazon")</f>
         <v>Amazon</v>
       </c>
       <c r="D22" s="1">
@@ -1311,27 +1299,27 @@
         <v>1</v>
       </c>
       <c r="F22" s="3">
-        <v>12.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="1"/>
-        <v>12.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="2"/>
-        <v>12.99</v>
+        <v>18.989999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="2" t="str">
-        <f>HYPERLINK("https://www.digikey.com/products/en?keywords=839-1146-ND", "10-01095")</f>
-        <v>10-01095</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f>HYPERLINK("https://www.amazon.com/HDE-Synthesizer-Microphone-Instrument-Converter/dp/B00D3QFHN8/ref=sr_1_7?ie=UTF8&amp;qid=1527187759&amp;sr=8-7&amp;keywords=USB+to+MIDI+cable&amp;dpID=413fQXN0jlL&amp;preST=_SY300_QL70_&amp;dpSrc=srch#customerReviews", "Amazon")</f>
+        <v>Amazon</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1341,108 +1329,77 @@
         <v>1</v>
       </c>
       <c r="F23" s="3">
-        <f>IF(E23 &lt; 10, 2.9, IF(E23 &lt; 25, 2.788, IF(E23 &lt; 50, 2.5552, IF(E23 &lt; 100, 2.4392, IF(E23 &lt; 250, 2.323, IF(E23 &lt; 500, 2.03264, IF(E23 &lt; 1000, 1.97456, IF(E23 &lt; 2500, 1.68418, 1.56802))))))))</f>
-        <v>2.9</v>
+        <v>9</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="1"/>
-        <v>2.9</v>
+        <v>9</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" si="2"/>
-        <v>2.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f>HYPERLINK("https://www.amazon.com/HDE-Synthesizer-Microphone-Instrument-Converter/dp/B00D3QFHN8/ref=sr_1_7?ie=UTF8&amp;qid=1527187759&amp;sr=8-7&amp;keywords=USB+to+MIDI+cable&amp;dpID=413fQXN0jlL&amp;preST=_SY300_QL70_&amp;dpSrc=srch#customerReviews", "Amazon")</f>
+        <f>HYPERLINK("https://www.amazon.com/J-Deal-Micro-Helicopter-Airplane-Controls/dp/B015H5AVZG/ref=sr_1_23_sspa?ie=UTF8&amp;qid=1519887306&amp;sr=8-23-spons&amp;keywords=tower+pro+micro+servo+9g&amp;psc=1", "Amazon")</f>
         <v>Amazon</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F24" s="3">
-        <v>9</v>
+        <v>1.36</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6.8000000000000007</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>6.8000000000000007</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="2" t="str">
-        <f>HYPERLINK("https://www.amazon.com/J-Deal-Micro-Helicopter-Airplane-Controls/dp/B015H5AVZG/ref=sr_1_23_sspa?ie=UTF8&amp;qid=1519887306&amp;sr=8-23-spons&amp;keywords=tower+pro+micro+servo+9g&amp;psc=1", "Amazon")</f>
-        <v>Amazon</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1.36</v>
-      </c>
+      <c r="B25" s="4"/>
+      <c r="D25" s="6">
+        <f>SUBTOTAL(109,Table2[Quantity/Jim Unit])</f>
+        <v>36</v>
+      </c>
+      <c r="E25" s="6">
+        <f>SUBTOTAL(109,Table2[Quantity/Total])</f>
+        <v>36</v>
+      </c>
+      <c r="F25" s="3"/>
       <c r="G25" s="3">
-        <f t="shared" si="1"/>
-        <v>6.8000000000000007</v>
+        <f>SUBTOTAL(109,Table2[Price/Jim Unit])</f>
+        <v>53.679999999999993</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="2"/>
-        <v>6.8000000000000007</v>
+        <f>SUBTOTAL(109,Table2[Price/Total])</f>
+        <v>53.679999999999993</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="D26" s="6">
-        <f>SUBTOTAL(109,Table2[Quantity/Jim Unit])</f>
-        <v>37</v>
-      </c>
-      <c r="E26" s="6">
-        <f>SUBTOTAL(109,Table2[Quantity/Total])</f>
-        <v>37</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3">
-        <f>SUBTOTAL(109,Table2[Price/Jim Unit])</f>
-        <v>50.2</v>
-      </c>
-      <c r="H26" s="3">
-        <f>SUBTOTAL(109,Table2[Price/Total])</f>
-        <v>50.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F25">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="F2:F24">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1455,8 +1412,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
-    <cfRule type="dataBar" priority="11">
+  <conditionalFormatting sqref="G2:G24">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1469,8 +1426,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="H2:H24">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1501,7 +1458,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F25</xm:sqref>
+          <xm:sqref>F2:F24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{11D47146-1F74-44D6-8B4E-88EBC93FA04D}">
@@ -1514,7 +1471,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G2:G25</xm:sqref>
+          <xm:sqref>G2:G24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C73A1683-4BBE-44F6-A587-83070DB74B75}">
@@ -1527,7 +1484,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H2:H25</xm:sqref>
+          <xm:sqref>H2:H24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>